<commit_message>
Adicionando dados de uma lista em uma planilha
métodos para adicionar informações de uma lista em uma planilha com comandos "for" e .cell do openpyxl
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="teste" sheetId="1" state="visible" r:id="rId1"/>
@@ -414,14 +414,1034 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Primeira célula preenchida</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Segunda Célula preenchida</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="n">
+        <v>3</v>
+      </c>
+      <c r="O3" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3</v>
+      </c>
+      <c r="R3" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4</v>
+      </c>
+      <c r="S4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>5</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" t="n">
+        <v>5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>5</v>
+      </c>
+      <c r="R5" t="n">
+        <v>5</v>
+      </c>
+      <c r="S5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" t="n">
+        <v>6</v>
+      </c>
+      <c r="K6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6</v>
+      </c>
+      <c r="M6" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O6" t="n">
+        <v>6</v>
+      </c>
+      <c r="P6" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>6</v>
+      </c>
+      <c r="R6" t="n">
+        <v>6</v>
+      </c>
+      <c r="S6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>7</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7</v>
+      </c>
+      <c r="L7" t="n">
+        <v>7</v>
+      </c>
+      <c r="M7" t="n">
+        <v>7</v>
+      </c>
+      <c r="N7" t="n">
+        <v>7</v>
+      </c>
+      <c r="O7" t="n">
+        <v>7</v>
+      </c>
+      <c r="P7" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>7</v>
+      </c>
+      <c r="R7" t="n">
+        <v>7</v>
+      </c>
+      <c r="S7" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" t="n">
+        <v>8</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8</v>
+      </c>
+      <c r="L8" t="n">
+        <v>8</v>
+      </c>
+      <c r="M8" t="n">
+        <v>8</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" t="n">
+        <v>8</v>
+      </c>
+      <c r="P8" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>8</v>
+      </c>
+      <c r="R8" t="n">
+        <v>8</v>
+      </c>
+      <c r="S8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9</v>
+      </c>
+      <c r="H9" t="n">
+        <v>9</v>
+      </c>
+      <c r="I9" t="n">
+        <v>9</v>
+      </c>
+      <c r="J9" t="n">
+        <v>9</v>
+      </c>
+      <c r="K9" t="n">
+        <v>9</v>
+      </c>
+      <c r="L9" t="n">
+        <v>9</v>
+      </c>
+      <c r="M9" t="n">
+        <v>9</v>
+      </c>
+      <c r="N9" t="n">
+        <v>9</v>
+      </c>
+      <c r="O9" t="n">
+        <v>9</v>
+      </c>
+      <c r="P9" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>9</v>
+      </c>
+      <c r="R9" t="n">
+        <v>9</v>
+      </c>
+      <c r="S9" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" t="n">
+        <v>10</v>
+      </c>
+      <c r="J10" t="n">
+        <v>10</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="n">
+        <v>10</v>
+      </c>
+      <c r="M10" t="n">
+        <v>10</v>
+      </c>
+      <c r="N10" t="n">
+        <v>10</v>
+      </c>
+      <c r="O10" t="n">
+        <v>10</v>
+      </c>
+      <c r="P10" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>10</v>
+      </c>
+      <c r="R10" t="n">
+        <v>10</v>
+      </c>
+      <c r="S10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" t="n">
+        <v>11</v>
+      </c>
+      <c r="D11" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" t="n">
+        <v>11</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11</v>
+      </c>
+      <c r="G11" t="n">
+        <v>11</v>
+      </c>
+      <c r="H11" t="n">
+        <v>11</v>
+      </c>
+      <c r="I11" t="n">
+        <v>11</v>
+      </c>
+      <c r="J11" t="n">
+        <v>11</v>
+      </c>
+      <c r="K11" t="n">
+        <v>11</v>
+      </c>
+      <c r="L11" t="n">
+        <v>11</v>
+      </c>
+      <c r="M11" t="n">
+        <v>11</v>
+      </c>
+      <c r="N11" t="n">
+        <v>11</v>
+      </c>
+      <c r="O11" t="n">
+        <v>11</v>
+      </c>
+      <c r="P11" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>11</v>
+      </c>
+      <c r="R11" t="n">
+        <v>11</v>
+      </c>
+      <c r="S11" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" t="n">
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>12</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12</v>
+      </c>
+      <c r="I12" t="n">
+        <v>12</v>
+      </c>
+      <c r="J12" t="n">
+        <v>12</v>
+      </c>
+      <c r="K12" t="n">
+        <v>12</v>
+      </c>
+      <c r="L12" t="n">
+        <v>12</v>
+      </c>
+      <c r="M12" t="n">
+        <v>12</v>
+      </c>
+      <c r="N12" t="n">
+        <v>12</v>
+      </c>
+      <c r="O12" t="n">
+        <v>12</v>
+      </c>
+      <c r="P12" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>12</v>
+      </c>
+      <c r="R12" t="n">
+        <v>12</v>
+      </c>
+      <c r="S12" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="n">
+        <v>13</v>
+      </c>
+      <c r="C13" t="n">
+        <v>13</v>
+      </c>
+      <c r="D13" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>13</v>
+      </c>
+      <c r="F13" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" t="n">
+        <v>13</v>
+      </c>
+      <c r="H13" t="n">
+        <v>13</v>
+      </c>
+      <c r="I13" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" t="n">
+        <v>13</v>
+      </c>
+      <c r="K13" t="n">
+        <v>13</v>
+      </c>
+      <c r="L13" t="n">
+        <v>13</v>
+      </c>
+      <c r="M13" t="n">
+        <v>13</v>
+      </c>
+      <c r="N13" t="n">
+        <v>13</v>
+      </c>
+      <c r="O13" t="n">
+        <v>13</v>
+      </c>
+      <c r="P13" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>13</v>
+      </c>
+      <c r="R13" t="n">
+        <v>13</v>
+      </c>
+      <c r="S13" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>14</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14</v>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="n">
+        <v>14</v>
+      </c>
+      <c r="F14" t="n">
+        <v>14</v>
+      </c>
+      <c r="G14" t="n">
+        <v>14</v>
+      </c>
+      <c r="H14" t="n">
+        <v>14</v>
+      </c>
+      <c r="I14" t="n">
+        <v>14</v>
+      </c>
+      <c r="J14" t="n">
+        <v>14</v>
+      </c>
+      <c r="K14" t="n">
+        <v>14</v>
+      </c>
+      <c r="L14" t="n">
+        <v>14</v>
+      </c>
+      <c r="M14" t="n">
+        <v>14</v>
+      </c>
+      <c r="N14" t="n">
+        <v>14</v>
+      </c>
+      <c r="O14" t="n">
+        <v>14</v>
+      </c>
+      <c r="P14" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>14</v>
+      </c>
+      <c r="R14" t="n">
+        <v>14</v>
+      </c>
+      <c r="S14" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+      <c r="B15" t="n">
+        <v>15</v>
+      </c>
+      <c r="C15" t="n">
+        <v>15</v>
+      </c>
+      <c r="D15" t="n">
+        <v>15</v>
+      </c>
+      <c r="E15" t="n">
+        <v>15</v>
+      </c>
+      <c r="F15" t="n">
+        <v>15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" t="n">
+        <v>15</v>
+      </c>
+      <c r="I15" t="n">
+        <v>15</v>
+      </c>
+      <c r="J15" t="n">
+        <v>15</v>
+      </c>
+      <c r="K15" t="n">
+        <v>15</v>
+      </c>
+      <c r="L15" t="n">
+        <v>15</v>
+      </c>
+      <c r="M15" t="n">
+        <v>15</v>
+      </c>
+      <c r="N15" t="n">
+        <v>15</v>
+      </c>
+      <c r="O15" t="n">
+        <v>15</v>
+      </c>
+      <c r="P15" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>15</v>
+      </c>
+      <c r="R15" t="n">
+        <v>15</v>
+      </c>
+      <c r="S15" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>16</v>
+      </c>
+      <c r="B16" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" t="n">
+        <v>16</v>
+      </c>
+      <c r="D16" t="n">
+        <v>16</v>
+      </c>
+      <c r="E16" t="n">
+        <v>16</v>
+      </c>
+      <c r="F16" t="n">
+        <v>16</v>
+      </c>
+      <c r="G16" t="n">
+        <v>16</v>
+      </c>
+      <c r="H16" t="n">
+        <v>16</v>
+      </c>
+      <c r="I16" t="n">
+        <v>16</v>
+      </c>
+      <c r="J16" t="n">
+        <v>16</v>
+      </c>
+      <c r="K16" t="n">
+        <v>16</v>
+      </c>
+      <c r="L16" t="n">
+        <v>16</v>
+      </c>
+      <c r="M16" t="n">
+        <v>16</v>
+      </c>
+      <c r="N16" t="n">
+        <v>16</v>
+      </c>
+      <c r="O16" t="n">
+        <v>16</v>
+      </c>
+      <c r="P16" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>16</v>
+      </c>
+      <c r="R16" t="n">
+        <v>16</v>
+      </c>
+      <c r="S16" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B17" t="n">
+        <v>17</v>
+      </c>
+      <c r="C17" t="n">
+        <v>17</v>
+      </c>
+      <c r="D17" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" t="n">
+        <v>17</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H17" t="n">
+        <v>17</v>
+      </c>
+      <c r="I17" t="n">
+        <v>17</v>
+      </c>
+      <c r="J17" t="n">
+        <v>17</v>
+      </c>
+      <c r="K17" t="n">
+        <v>17</v>
+      </c>
+      <c r="L17" t="n">
+        <v>17</v>
+      </c>
+      <c r="M17" t="n">
+        <v>17</v>
+      </c>
+      <c r="N17" t="n">
+        <v>17</v>
+      </c>
+      <c r="O17" t="n">
+        <v>17</v>
+      </c>
+      <c r="P17" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>17</v>
+      </c>
+      <c r="R17" t="n">
+        <v>17</v>
+      </c>
+      <c r="S17" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>18</v>
+      </c>
+      <c r="B18" t="n">
+        <v>18</v>
+      </c>
+      <c r="C18" t="n">
+        <v>18</v>
+      </c>
+      <c r="D18" t="n">
+        <v>18</v>
+      </c>
+      <c r="E18" t="n">
+        <v>18</v>
+      </c>
+      <c r="F18" t="n">
+        <v>18</v>
+      </c>
+      <c r="G18" t="n">
+        <v>18</v>
+      </c>
+      <c r="H18" t="n">
+        <v>18</v>
+      </c>
+      <c r="I18" t="n">
+        <v>18</v>
+      </c>
+      <c r="J18" t="n">
+        <v>18</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18</v>
+      </c>
+      <c r="L18" t="n">
+        <v>18</v>
+      </c>
+      <c r="M18" t="n">
+        <v>18</v>
+      </c>
+      <c r="N18" t="n">
+        <v>18</v>
+      </c>
+      <c r="O18" t="n">
+        <v>18</v>
+      </c>
+      <c r="P18" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>18</v>
+      </c>
+      <c r="R18" t="n">
+        <v>18</v>
+      </c>
+      <c r="S18" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>19</v>
+      </c>
+      <c r="C19" t="n">
+        <v>19</v>
+      </c>
+      <c r="D19" t="n">
+        <v>19</v>
+      </c>
+      <c r="E19" t="n">
+        <v>19</v>
+      </c>
+      <c r="F19" t="n">
+        <v>19</v>
+      </c>
+      <c r="G19" t="n">
+        <v>19</v>
+      </c>
+      <c r="H19" t="n">
+        <v>19</v>
+      </c>
+      <c r="I19" t="n">
+        <v>19</v>
+      </c>
+      <c r="J19" t="n">
+        <v>19</v>
+      </c>
+      <c r="K19" t="n">
+        <v>19</v>
+      </c>
+      <c r="L19" t="n">
+        <v>19</v>
+      </c>
+      <c r="M19" t="n">
+        <v>19</v>
+      </c>
+      <c r="N19" t="n">
+        <v>19</v>
+      </c>
+      <c r="O19" t="n">
+        <v>19</v>
+      </c>
+      <c r="P19" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>19</v>
+      </c>
+      <c r="R19" t="n">
+        <v>19</v>
+      </c>
+      <c r="S19" t="n">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -433,14 +1453,83 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Código</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Material de Limpeza</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Material de Consumo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Matéria Primo</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>